<commit_message>
progress on proj 2
asdfasdf
</commit_message>
<xml_diff>
--- a/projects/project-2/assignment/src/aircraft_data.xlsx
+++ b/projects/project-2/assignment/src/aircraft_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\FAA\Drupal\Airports\Engineering, Design, &amp; Construction\Aircraft Characteristics Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\Ontology-Tradecraft\projects\project-2\assignment\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3528D2D9-1EA8-4CE3-9F8C-0DF0E568D119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C04BE0-1C5D-41ED-8310-A0535C392D78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{852B0E64-BCCC-407E-85AF-9EDDBE8136BD}"/>
+    <workbookView xWindow="-37" yWindow="0" windowWidth="19185" windowHeight="10162" activeTab="1" xr2:uid="{852B0E64-BCCC-407E-85AF-9EDDBE8136BD}"/>
   </bookViews>
   <sheets>
     <sheet name="ACD_Data" sheetId="1" r:id="rId1"/>
@@ -6526,7 +6526,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DAC96F04-B94D-467A-960C-7C5EEB455C42}" name="Table4" displayName="Table4" ref="A1:AO389" totalsRowShown="0" headerRowDxfId="45" dataDxfId="43" headerRowBorderDxfId="44" tableBorderDxfId="42" totalsRowBorderDxfId="41">
-  <autoFilter ref="A1:AO389" xr:uid="{DAC96F04-B94D-467A-960C-7C5EEB455C42}"/>
+  <autoFilter ref="A1:AO389" xr:uid="{DAC96F04-B94D-467A-960C-7C5EEB455C42}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="A320"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AO389">
     <sortCondition ref="A2:A389"/>
   </sortState>
@@ -6578,9 +6584,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -6618,7 +6624,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -6724,7 +6730,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6866,7 +6872,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -6876,61 +6882,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B2C235D-FDEC-42F2-8FD4-154978FFF057}">
   <dimension ref="A1:BD389"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="AH12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D215" sqref="D215"/>
+      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" style="18" customWidth="1"/>
-    <col min="2" max="2" width="31.44140625" style="18" customWidth="1"/>
-    <col min="3" max="3" width="25.77734375" style="18" customWidth="1"/>
+    <col min="1" max="1" width="13.796875" style="18" customWidth="1"/>
+    <col min="2" max="2" width="31.46484375" style="18" customWidth="1"/>
+    <col min="3" max="3" width="25.796875" style="18" customWidth="1"/>
     <col min="4" max="4" width="67.6640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.44140625" style="18" customWidth="1"/>
-    <col min="6" max="6" width="24.44140625" style="18" customWidth="1"/>
-    <col min="7" max="7" width="15.77734375" style="18" customWidth="1"/>
-    <col min="8" max="8" width="16.44140625" style="18" customWidth="1"/>
+    <col min="5" max="5" width="38.46484375" style="18" customWidth="1"/>
+    <col min="6" max="6" width="24.46484375" style="18" customWidth="1"/>
+    <col min="7" max="7" width="15.796875" style="18" customWidth="1"/>
+    <col min="8" max="8" width="16.46484375" style="18" customWidth="1"/>
     <col min="9" max="9" width="18.6640625" style="18" customWidth="1"/>
     <col min="10" max="10" width="19" style="18" customWidth="1"/>
-    <col min="11" max="12" width="9.109375" style="18"/>
+    <col min="11" max="12" width="9.1328125" style="18"/>
     <col min="13" max="13" width="24.6640625" style="18" customWidth="1"/>
     <col min="14" max="14" width="32" style="18" customWidth="1"/>
     <col min="15" max="15" width="32.33203125" style="18" customWidth="1"/>
-    <col min="16" max="16" width="43.77734375" style="42" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="43.796875" style="42" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="35" style="42" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.44140625" style="42" customWidth="1"/>
+    <col min="18" max="18" width="12.46484375" style="42" customWidth="1"/>
     <col min="19" max="19" width="26" style="42" customWidth="1"/>
-    <col min="20" max="20" width="16.44140625" style="42" customWidth="1"/>
+    <col min="20" max="20" width="16.46484375" style="42" customWidth="1"/>
     <col min="21" max="21" width="28.33203125" style="42" customWidth="1"/>
-    <col min="22" max="22" width="23.77734375" style="42" customWidth="1"/>
+    <col min="22" max="22" width="23.796875" style="42" customWidth="1"/>
     <col min="23" max="23" width="23.33203125" style="43" customWidth="1"/>
     <col min="24" max="24" width="22" style="43" customWidth="1"/>
-    <col min="25" max="25" width="21.109375" style="18" customWidth="1"/>
-    <col min="26" max="26" width="13.44140625" style="18" customWidth="1"/>
-    <col min="27" max="27" width="20.109375" style="42" customWidth="1"/>
-    <col min="28" max="28" width="17.44140625" style="18" customWidth="1"/>
+    <col min="25" max="25" width="21.1328125" style="18" customWidth="1"/>
+    <col min="26" max="26" width="13.46484375" style="18" customWidth="1"/>
+    <col min="27" max="27" width="20.1328125" style="42" customWidth="1"/>
+    <col min="28" max="28" width="17.46484375" style="18" customWidth="1"/>
     <col min="29" max="29" width="15.33203125" style="18" customWidth="1"/>
-    <col min="30" max="30" width="15.44140625" style="18" customWidth="1"/>
+    <col min="30" max="30" width="15.46484375" style="18" customWidth="1"/>
     <col min="31" max="31" width="32.33203125" style="23" customWidth="1"/>
-    <col min="32" max="32" width="36.109375" style="18" customWidth="1"/>
-    <col min="33" max="33" width="32.44140625" style="18" customWidth="1"/>
-    <col min="34" max="34" width="21.44140625" style="18" customWidth="1"/>
-    <col min="35" max="35" width="9.109375" style="18"/>
+    <col min="32" max="32" width="36.1328125" style="18" customWidth="1"/>
+    <col min="33" max="33" width="32.46484375" style="18" customWidth="1"/>
+    <col min="34" max="34" width="21.46484375" style="18" customWidth="1"/>
+    <col min="35" max="35" width="9.1328125" style="18"/>
     <col min="36" max="36" width="9.6640625" style="18" customWidth="1"/>
     <col min="37" max="37" width="16" style="18" customWidth="1"/>
     <col min="38" max="38" width="22" style="43" customWidth="1"/>
     <col min="39" max="39" width="26.33203125" style="43" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="111.77734375" style="18" customWidth="1"/>
-    <col min="41" max="41" width="14.109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="42" max="47" width="9.109375" style="18"/>
-    <col min="48" max="48" width="52.44140625" style="18" customWidth="1"/>
-    <col min="49" max="16384" width="9.109375" style="18"/>
+    <col min="40" max="40" width="111.796875" style="18" customWidth="1"/>
+    <col min="41" max="41" width="14.1328125" style="18" bestFit="1" customWidth="1"/>
+    <col min="42" max="47" width="9.1328125" style="18"/>
+    <col min="48" max="48" width="52.46484375" style="18" customWidth="1"/>
+    <col min="49" max="16384" width="9.1328125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.5">
       <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
@@ -7055,7 +7061,7 @@
         <v>1403</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A2" s="29" t="s">
         <v>39</v>
       </c>
@@ -7164,7 +7170,7 @@
       <c r="AN2" s="19"/>
       <c r="AO2" s="20"/>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A3" s="29" t="s">
         <v>57</v>
       </c>
@@ -7273,7 +7279,7 @@
       <c r="AN3" s="19"/>
       <c r="AO3" s="20"/>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A4" s="29" t="s">
         <v>65</v>
       </c>
@@ -7384,7 +7390,7 @@
       </c>
       <c r="AO4" s="20"/>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A5" s="29" t="s">
         <v>71</v>
       </c>
@@ -7495,7 +7501,7 @@
       </c>
       <c r="AO5" s="20"/>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A6" s="29" t="s">
         <v>75</v>
       </c>
@@ -7606,7 +7612,7 @@
       </c>
       <c r="AO6" s="20"/>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A7" s="29" t="s">
         <v>78</v>
       </c>
@@ -7717,7 +7723,7 @@
       </c>
       <c r="AO7" s="20"/>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A8" s="29" t="s">
         <v>83</v>
       </c>
@@ -7828,7 +7834,7 @@
       </c>
       <c r="AO8" s="20"/>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A9" s="29" t="s">
         <v>86</v>
       </c>
@@ -7939,7 +7945,7 @@
       </c>
       <c r="AO9" s="20"/>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A10" s="29" t="s">
         <v>89</v>
       </c>
@@ -8050,7 +8056,7 @@
       </c>
       <c r="AO10" s="20"/>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A11" s="29" t="s">
         <v>92</v>
       </c>
@@ -8163,7 +8169,7 @@
       </c>
       <c r="AO11" s="20"/>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.5">
       <c r="A12" s="29" t="s">
         <v>95</v>
       </c>
@@ -8276,7 +8282,7 @@
       </c>
       <c r="AO12" s="20"/>
     </row>
-    <row r="13" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:41" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A13" s="29" t="s">
         <v>98</v>
       </c>
@@ -8397,7 +8403,7 @@
       </c>
       <c r="AO13" s="20"/>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A14" s="29" t="s">
         <v>102</v>
       </c>
@@ -8508,7 +8514,7 @@
       </c>
       <c r="AO14" s="20"/>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A15" s="29" t="s">
         <v>107</v>
       </c>
@@ -8619,7 +8625,7 @@
       </c>
       <c r="AO15" s="20"/>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A16" s="29" t="s">
         <v>110</v>
       </c>
@@ -8728,7 +8734,7 @@
       <c r="AN16" s="19"/>
       <c r="AO16" s="20"/>
     </row>
-    <row r="17" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:56" hidden="1" x14ac:dyDescent="0.5">
       <c r="A17" s="29" t="s">
         <v>113</v>
       </c>
@@ -8837,7 +8843,7 @@
       <c r="AN17" s="19"/>
       <c r="AO17" s="20"/>
     </row>
-    <row r="18" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:56" hidden="1" x14ac:dyDescent="0.5">
       <c r="A18" s="29" t="s">
         <v>115</v>
       </c>
@@ -8948,7 +8954,7 @@
       </c>
       <c r="AO18" s="20"/>
     </row>
-    <row r="19" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:56" hidden="1" x14ac:dyDescent="0.5">
       <c r="A19" s="29" t="s">
         <v>118</v>
       </c>
@@ -9057,7 +9063,7 @@
       <c r="AN19" s="19"/>
       <c r="AO19" s="20"/>
     </row>
-    <row r="20" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:56" hidden="1" x14ac:dyDescent="0.5">
       <c r="A20" s="29" t="s">
         <v>122</v>
       </c>
@@ -9166,7 +9172,7 @@
       <c r="AN20" s="19"/>
       <c r="AO20" s="20"/>
     </row>
-    <row r="21" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:56" hidden="1" x14ac:dyDescent="0.5">
       <c r="A21" s="29" t="s">
         <v>125</v>
       </c>
@@ -9275,7 +9281,7 @@
       <c r="AN21" s="19"/>
       <c r="AO21" s="20"/>
     </row>
-    <row r="22" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:56" hidden="1" x14ac:dyDescent="0.5">
       <c r="A22" s="29" t="s">
         <v>129</v>
       </c>
@@ -9384,7 +9390,7 @@
       <c r="AN22" s="19"/>
       <c r="AO22" s="20"/>
     </row>
-    <row r="23" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:56" hidden="1" x14ac:dyDescent="0.5">
       <c r="A23" s="29" t="s">
         <v>132</v>
       </c>
@@ -9497,7 +9503,7 @@
         <v>45571</v>
       </c>
     </row>
-    <row r="24" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:56" hidden="1" x14ac:dyDescent="0.5">
       <c r="A24" s="29" t="s">
         <v>135</v>
       </c>
@@ -9610,7 +9616,7 @@
         <v>45571</v>
       </c>
     </row>
-    <row r="25" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:56" hidden="1" x14ac:dyDescent="0.5">
       <c r="A25" s="29" t="s">
         <v>139</v>
       </c>
@@ -9723,7 +9729,7 @@
         <v>45571</v>
       </c>
     </row>
-    <row r="26" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:56" hidden="1" x14ac:dyDescent="0.5">
       <c r="A26" s="29" t="s">
         <v>144</v>
       </c>
@@ -9832,7 +9838,7 @@
       <c r="AN26" s="19"/>
       <c r="AO26" s="20"/>
     </row>
-    <row r="27" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:56" hidden="1" x14ac:dyDescent="0.5">
       <c r="A27" s="29" t="s">
         <v>148</v>
       </c>
@@ -9941,7 +9947,7 @@
       <c r="AN27" s="19"/>
       <c r="AO27" s="20"/>
     </row>
-    <row r="28" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:56" hidden="1" x14ac:dyDescent="0.5">
       <c r="A28" s="29" t="s">
         <v>157</v>
       </c>
@@ -10053,7 +10059,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="29" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:56" hidden="1" x14ac:dyDescent="0.5">
       <c r="A29" s="29" t="s">
         <v>162</v>
       </c>
@@ -10162,7 +10168,7 @@
       <c r="AN29" s="19"/>
       <c r="AO29" s="20"/>
     </row>
-    <row r="30" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:56" hidden="1" x14ac:dyDescent="0.5">
       <c r="A30" s="29" t="s">
         <v>165</v>
       </c>
@@ -10271,7 +10277,7 @@
       <c r="AN30" s="19"/>
       <c r="AO30" s="20"/>
     </row>
-    <row r="31" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:56" hidden="1" x14ac:dyDescent="0.5">
       <c r="A31" s="29" t="s">
         <v>169</v>
       </c>
@@ -10380,7 +10386,7 @@
       <c r="AN31" s="19"/>
       <c r="AO31" s="20"/>
     </row>
-    <row r="32" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:56" hidden="1" x14ac:dyDescent="0.5">
       <c r="A32" s="29" t="s">
         <v>172</v>
       </c>
@@ -10489,7 +10495,7 @@
       <c r="AN32" s="19"/>
       <c r="AO32" s="20"/>
     </row>
-    <row r="33" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A33" s="29" t="s">
         <v>174</v>
       </c>
@@ -10598,7 +10604,7 @@
       <c r="AN33" s="19"/>
       <c r="AO33" s="20"/>
     </row>
-    <row r="34" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A34" s="29" t="s">
         <v>177</v>
       </c>
@@ -10707,7 +10713,7 @@
       <c r="AN34" s="19"/>
       <c r="AO34" s="20"/>
     </row>
-    <row r="35" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A35" s="29" t="s">
         <v>180</v>
       </c>
@@ -10816,7 +10822,7 @@
       <c r="AN35" s="19"/>
       <c r="AO35" s="20"/>
     </row>
-    <row r="36" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A36" s="29" t="s">
         <v>183</v>
       </c>
@@ -10925,7 +10931,7 @@
       <c r="AN36" s="19"/>
       <c r="AO36" s="20"/>
     </row>
-    <row r="37" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A37" s="29" t="s">
         <v>187</v>
       </c>
@@ -11034,7 +11040,7 @@
       <c r="AN37" s="19"/>
       <c r="AO37" s="20"/>
     </row>
-    <row r="38" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A38" s="29" t="s">
         <v>190</v>
       </c>
@@ -11143,7 +11149,7 @@
       <c r="AN38" s="19"/>
       <c r="AO38" s="20"/>
     </row>
-    <row r="39" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A39" s="29" t="s">
         <v>194</v>
       </c>
@@ -11252,7 +11258,7 @@
       <c r="AN39" s="19"/>
       <c r="AO39" s="20"/>
     </row>
-    <row r="40" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A40" s="29" t="s">
         <v>197</v>
       </c>
@@ -11361,7 +11367,7 @@
       <c r="AN40" s="19"/>
       <c r="AO40" s="20"/>
     </row>
-    <row r="41" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A41" s="29" t="s">
         <v>202</v>
       </c>
@@ -11470,7 +11476,7 @@
       <c r="AN41" s="19"/>
       <c r="AO41" s="20"/>
     </row>
-    <row r="42" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A42" s="29" t="s">
         <v>205</v>
       </c>
@@ -11579,7 +11585,7 @@
       <c r="AN42" s="19"/>
       <c r="AO42" s="20"/>
     </row>
-    <row r="43" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A43" s="29" t="s">
         <v>211</v>
       </c>
@@ -11688,7 +11694,7 @@
       <c r="AN43" s="19"/>
       <c r="AO43" s="20"/>
     </row>
-    <row r="44" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A44" s="29" t="s">
         <v>215</v>
       </c>
@@ -11797,7 +11803,7 @@
       <c r="AN44" s="19"/>
       <c r="AO44" s="20"/>
     </row>
-    <row r="45" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A45" s="29" t="s">
         <v>219</v>
       </c>
@@ -11906,7 +11912,7 @@
       <c r="AN45" s="19"/>
       <c r="AO45" s="20"/>
     </row>
-    <row r="46" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A46" s="29" t="s">
         <v>222</v>
       </c>
@@ -12015,7 +12021,7 @@
       <c r="AN46" s="19"/>
       <c r="AO46" s="20"/>
     </row>
-    <row r="47" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A47" s="29" t="s">
         <v>224</v>
       </c>
@@ -12124,7 +12130,7 @@
       <c r="AN47" s="19"/>
       <c r="AO47" s="20"/>
     </row>
-    <row r="48" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A48" s="29" t="s">
         <v>226</v>
       </c>
@@ -12233,7 +12239,7 @@
       <c r="AN48" s="19"/>
       <c r="AO48" s="20"/>
     </row>
-    <row r="49" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A49" s="29" t="s">
         <v>229</v>
       </c>
@@ -12342,7 +12348,7 @@
       <c r="AN49" s="19"/>
       <c r="AO49" s="20"/>
     </row>
-    <row r="50" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A50" s="29" t="s">
         <v>232</v>
       </c>
@@ -12451,7 +12457,7 @@
       <c r="AN50" s="19"/>
       <c r="AO50" s="20"/>
     </row>
-    <row r="51" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A51" s="29" t="s">
         <v>235</v>
       </c>
@@ -12560,7 +12566,7 @@
       <c r="AN51" s="19"/>
       <c r="AO51" s="20"/>
     </row>
-    <row r="52" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A52" s="29" t="s">
         <v>238</v>
       </c>
@@ -12669,7 +12675,7 @@
       <c r="AN52" s="19"/>
       <c r="AO52" s="20"/>
     </row>
-    <row r="53" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A53" s="29" t="s">
         <v>241</v>
       </c>
@@ -12778,7 +12784,7 @@
       <c r="AN53" s="19"/>
       <c r="AO53" s="20"/>
     </row>
-    <row r="54" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A54" s="29" t="s">
         <v>244</v>
       </c>
@@ -12887,7 +12893,7 @@
       <c r="AN54" s="19"/>
       <c r="AO54" s="20"/>
     </row>
-    <row r="55" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A55" s="29" t="s">
         <v>248</v>
       </c>
@@ -12996,7 +13002,7 @@
       <c r="AN55" s="19"/>
       <c r="AO55" s="20"/>
     </row>
-    <row r="56" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A56" s="29" t="s">
         <v>252</v>
       </c>
@@ -13115,7 +13121,7 @@
       </c>
       <c r="AO56" s="20"/>
     </row>
-    <row r="57" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A57" s="29" t="s">
         <v>255</v>
       </c>
@@ -13224,7 +13230,7 @@
       <c r="AN57" s="19"/>
       <c r="AO57" s="20"/>
     </row>
-    <row r="58" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A58" s="29" t="s">
         <v>258</v>
       </c>
@@ -13333,7 +13339,7 @@
       <c r="AN58" s="19"/>
       <c r="AO58" s="20"/>
     </row>
-    <row r="59" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A59" s="29" t="s">
         <v>261</v>
       </c>
@@ -13442,7 +13448,7 @@
       <c r="AN59" s="19"/>
       <c r="AO59" s="20"/>
     </row>
-    <row r="60" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A60" s="29" t="s">
         <v>265</v>
       </c>
@@ -13561,7 +13567,7 @@
       </c>
       <c r="AO60" s="20"/>
     </row>
-    <row r="61" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A61" s="29" t="s">
         <v>270</v>
       </c>
@@ -13680,7 +13686,7 @@
       </c>
       <c r="AO61" s="20"/>
     </row>
-    <row r="62" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A62" s="29" t="s">
         <v>273</v>
       </c>
@@ -13799,7 +13805,7 @@
       </c>
       <c r="AO62" s="20"/>
     </row>
-    <row r="63" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A63" s="29" t="s">
         <v>276</v>
       </c>
@@ -13908,7 +13914,7 @@
       <c r="AN63" s="19"/>
       <c r="AO63" s="20"/>
     </row>
-    <row r="64" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A64" s="29" t="s">
         <v>280</v>
       </c>
@@ -14017,7 +14023,7 @@
       <c r="AN64" s="19"/>
       <c r="AO64" s="20"/>
     </row>
-    <row r="65" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A65" s="29" t="s">
         <v>283</v>
       </c>
@@ -14126,7 +14132,7 @@
       <c r="AN65" s="19"/>
       <c r="AO65" s="20"/>
     </row>
-    <row r="66" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A66" s="29" t="s">
         <v>286</v>
       </c>
@@ -14235,7 +14241,7 @@
       <c r="AN66" s="19"/>
       <c r="AO66" s="20"/>
     </row>
-    <row r="67" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A67" s="29" t="s">
         <v>289</v>
       </c>
@@ -14346,7 +14352,7 @@
       </c>
       <c r="AO67" s="20"/>
     </row>
-    <row r="68" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A68" s="29" t="s">
         <v>292</v>
       </c>
@@ -14455,7 +14461,7 @@
       <c r="AN68" s="19"/>
       <c r="AO68" s="20"/>
     </row>
-    <row r="69" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A69" s="29" t="s">
         <v>295</v>
       </c>
@@ -14566,7 +14572,7 @@
       <c r="AN69" s="19"/>
       <c r="AO69" s="20"/>
     </row>
-    <row r="70" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A70" s="29" t="s">
         <v>298</v>
       </c>
@@ -14677,7 +14683,7 @@
       </c>
       <c r="AO70" s="20"/>
     </row>
-    <row r="71" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A71" s="29" t="s">
         <v>301</v>
       </c>
@@ -14790,7 +14796,7 @@
       </c>
       <c r="AO71" s="20"/>
     </row>
-    <row r="72" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A72" s="29" t="s">
         <v>304</v>
       </c>
@@ -14901,7 +14907,7 @@
       </c>
       <c r="AO72" s="20"/>
     </row>
-    <row r="73" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A73" s="29" t="s">
         <v>307</v>
       </c>
@@ -15012,7 +15018,7 @@
       </c>
       <c r="AO73" s="20"/>
     </row>
-    <row r="74" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A74" s="29" t="s">
         <v>310</v>
       </c>
@@ -15125,7 +15131,7 @@
       </c>
       <c r="AO74" s="20"/>
     </row>
-    <row r="75" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A75" s="29" t="s">
         <v>313</v>
       </c>
@@ -15238,7 +15244,7 @@
       </c>
       <c r="AO75" s="20"/>
     </row>
-    <row r="76" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A76" s="29" t="s">
         <v>316</v>
       </c>
@@ -15359,7 +15365,7 @@
       </c>
       <c r="AO76" s="20"/>
     </row>
-    <row r="77" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A77" s="29" t="s">
         <v>319</v>
       </c>
@@ -15480,7 +15486,7 @@
       </c>
       <c r="AO77" s="20"/>
     </row>
-    <row r="78" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A78" s="29" t="s">
         <v>322</v>
       </c>
@@ -15589,7 +15595,7 @@
       <c r="AN78" s="19"/>
       <c r="AO78" s="20"/>
     </row>
-    <row r="79" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A79" s="29" t="s">
         <v>325</v>
       </c>
@@ -15698,7 +15704,7 @@
       <c r="AN79" s="19"/>
       <c r="AO79" s="20"/>
     </row>
-    <row r="80" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A80" s="29" t="s">
         <v>328</v>
       </c>
@@ -15807,7 +15813,7 @@
       <c r="AN80" s="19"/>
       <c r="AO80" s="20"/>
     </row>
-    <row r="81" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A81" s="29" t="s">
         <v>331</v>
       </c>
@@ -15918,7 +15924,7 @@
       </c>
       <c r="AO81" s="20"/>
     </row>
-    <row r="82" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A82" s="29" t="s">
         <v>334</v>
       </c>
@@ -16029,7 +16035,7 @@
       </c>
       <c r="AO82" s="20"/>
     </row>
-    <row r="83" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A83" s="29" t="s">
         <v>337</v>
       </c>
@@ -16140,7 +16146,7 @@
       <c r="AN83" s="19"/>
       <c r="AO83" s="20"/>
     </row>
-    <row r="84" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A84" s="29" t="s">
         <v>340</v>
       </c>
@@ -16251,7 +16257,7 @@
       <c r="AN84" s="19"/>
       <c r="AO84" s="20"/>
     </row>
-    <row r="85" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A85" s="29" t="s">
         <v>343</v>
       </c>
@@ -16360,7 +16366,7 @@
       <c r="AN85" s="19"/>
       <c r="AO85" s="20"/>
     </row>
-    <row r="86" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A86" s="29" t="s">
         <v>346</v>
       </c>
@@ -16471,7 +16477,7 @@
       <c r="AN86" s="19"/>
       <c r="AO86" s="20"/>
     </row>
-    <row r="87" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A87" s="29" t="s">
         <v>349</v>
       </c>
@@ -16580,7 +16586,7 @@
       <c r="AN87" s="19"/>
       <c r="AO87" s="20"/>
     </row>
-    <row r="88" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A88" s="29" t="s">
         <v>352</v>
       </c>
@@ -16691,7 +16697,7 @@
       </c>
       <c r="AO88" s="20"/>
     </row>
-    <row r="89" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A89" s="29" t="s">
         <v>355</v>
       </c>
@@ -16802,7 +16808,7 @@
       </c>
       <c r="AO89" s="20"/>
     </row>
-    <row r="90" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A90" s="29" t="s">
         <v>358</v>
       </c>
@@ -16913,7 +16919,7 @@
       </c>
       <c r="AO90" s="20"/>
     </row>
-    <row r="91" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A91" s="29" t="s">
         <v>361</v>
       </c>
@@ -17024,7 +17030,7 @@
       </c>
       <c r="AO91" s="20"/>
     </row>
-    <row r="92" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A92" s="29" t="s">
         <v>363</v>
       </c>
@@ -17135,7 +17141,7 @@
       </c>
       <c r="AO92" s="20"/>
     </row>
-    <row r="93" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A93" s="29" t="s">
         <v>366</v>
       </c>
@@ -17246,7 +17252,7 @@
       </c>
       <c r="AO93" s="20"/>
     </row>
-    <row r="94" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A94" s="29" t="s">
         <v>369</v>
       </c>
@@ -17365,7 +17371,7 @@
       </c>
       <c r="AO94" s="20"/>
     </row>
-    <row r="95" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A95" s="29" t="s">
         <v>373</v>
       </c>
@@ -17484,7 +17490,7 @@
       </c>
       <c r="AO95" s="20"/>
     </row>
-    <row r="96" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A96" s="29" t="s">
         <v>376</v>
       </c>
@@ -17595,7 +17601,7 @@
       </c>
       <c r="AO96" s="20"/>
     </row>
-    <row r="97" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A97" s="29" t="s">
         <v>380</v>
       </c>
@@ -17704,7 +17710,7 @@
       <c r="AN97" s="19"/>
       <c r="AO97" s="20"/>
     </row>
-    <row r="98" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A98" s="29" t="s">
         <v>384</v>
       </c>
@@ -17815,7 +17821,7 @@
       </c>
       <c r="AO98" s="20"/>
     </row>
-    <row r="99" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A99" s="29" t="s">
         <v>388</v>
       </c>
@@ -17924,7 +17930,7 @@
       <c r="AN99" s="19"/>
       <c r="AO99" s="20"/>
     </row>
-    <row r="100" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A100" s="29" t="s">
         <v>391</v>
       </c>
@@ -18033,7 +18039,7 @@
       <c r="AN100" s="19"/>
       <c r="AO100" s="20"/>
     </row>
-    <row r="101" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A101" s="29" t="s">
         <v>394</v>
       </c>
@@ -18142,7 +18148,7 @@
       <c r="AN101" s="19"/>
       <c r="AO101" s="20"/>
     </row>
-    <row r="102" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A102" s="29" t="s">
         <v>397</v>
       </c>
@@ -18251,7 +18257,7 @@
       <c r="AN102" s="19"/>
       <c r="AO102" s="20"/>
     </row>
-    <row r="103" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A103" s="29" t="s">
         <v>400</v>
       </c>
@@ -18362,7 +18368,7 @@
       </c>
       <c r="AO103" s="20"/>
     </row>
-    <row r="104" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A104" s="29" t="s">
         <v>403</v>
       </c>
@@ -18471,7 +18477,7 @@
       <c r="AN104" s="19"/>
       <c r="AO104" s="20"/>
     </row>
-    <row r="105" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A105" s="29" t="s">
         <v>406</v>
       </c>
@@ -18580,7 +18586,7 @@
       <c r="AN105" s="19"/>
       <c r="AO105" s="20"/>
     </row>
-    <row r="106" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A106" s="29" t="s">
         <v>408</v>
       </c>
@@ -18691,7 +18697,7 @@
       </c>
       <c r="AO106" s="20"/>
     </row>
-    <row r="107" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A107" s="29" t="s">
         <v>412</v>
       </c>
@@ -18800,7 +18806,7 @@
       <c r="AN107" s="19"/>
       <c r="AO107" s="20"/>
     </row>
-    <row r="108" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A108" s="29" t="s">
         <v>415</v>
       </c>
@@ -18909,7 +18915,7 @@
       <c r="AN108" s="19"/>
       <c r="AO108" s="20"/>
     </row>
-    <row r="109" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A109" s="29" t="s">
         <v>418</v>
       </c>
@@ -19018,7 +19024,7 @@
       <c r="AN109" s="19"/>
       <c r="AO109" s="20"/>
     </row>
-    <row r="110" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A110" s="29" t="s">
         <v>421</v>
       </c>
@@ -19127,7 +19133,7 @@
       <c r="AN110" s="19"/>
       <c r="AO110" s="20"/>
     </row>
-    <row r="111" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A111" s="29" t="s">
         <v>425</v>
       </c>
@@ -19236,7 +19242,7 @@
       <c r="AN111" s="19"/>
       <c r="AO111" s="20"/>
     </row>
-    <row r="112" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A112" s="29" t="s">
         <v>428</v>
       </c>
@@ -19345,7 +19351,7 @@
       <c r="AN112" s="19"/>
       <c r="AO112" s="20"/>
     </row>
-    <row r="113" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A113" s="29" t="s">
         <v>431</v>
       </c>
@@ -19454,7 +19460,7 @@
       <c r="AN113" s="19"/>
       <c r="AO113" s="20"/>
     </row>
-    <row r="114" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A114" s="29" t="s">
         <v>434</v>
       </c>
@@ -19563,7 +19569,7 @@
       <c r="AN114" s="19"/>
       <c r="AO114" s="20"/>
     </row>
-    <row r="115" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A115" s="29" t="s">
         <v>436</v>
       </c>
@@ -19672,7 +19678,7 @@
       <c r="AN115" s="19"/>
       <c r="AO115" s="20"/>
     </row>
-    <row r="116" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A116" s="29" t="s">
         <v>438</v>
       </c>
@@ -19781,7 +19787,7 @@
       <c r="AN116" s="19"/>
       <c r="AO116" s="20"/>
     </row>
-    <row r="117" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A117" s="29" t="s">
         <v>440</v>
       </c>
@@ -19890,7 +19896,7 @@
       <c r="AN117" s="19"/>
       <c r="AO117" s="20"/>
     </row>
-    <row r="118" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A118" s="29" t="s">
         <v>443</v>
       </c>
@@ -19999,7 +20005,7 @@
       <c r="AN118" s="19"/>
       <c r="AO118" s="20"/>
     </row>
-    <row r="119" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A119" s="29" t="s">
         <v>445</v>
       </c>
@@ -20108,7 +20114,7 @@
       <c r="AN119" s="19"/>
       <c r="AO119" s="20"/>
     </row>
-    <row r="120" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A120" s="29" t="s">
         <v>448</v>
       </c>
@@ -20217,7 +20223,7 @@
       <c r="AN120" s="19"/>
       <c r="AO120" s="20"/>
     </row>
-    <row r="121" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A121" s="29" t="s">
         <v>451</v>
       </c>
@@ -20326,7 +20332,7 @@
       <c r="AN121" s="19"/>
       <c r="AO121" s="20"/>
     </row>
-    <row r="122" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A122" s="29" t="s">
         <v>454</v>
       </c>
@@ -20435,7 +20441,7 @@
       <c r="AN122" s="19"/>
       <c r="AO122" s="20"/>
     </row>
-    <row r="123" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A123" s="29" t="s">
         <v>457</v>
       </c>
@@ -20544,7 +20550,7 @@
       <c r="AN123" s="19"/>
       <c r="AO123" s="20"/>
     </row>
-    <row r="124" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A124" s="29" t="s">
         <v>460</v>
       </c>
@@ -20653,7 +20659,7 @@
       <c r="AN124" s="19"/>
       <c r="AO124" s="20"/>
     </row>
-    <row r="125" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A125" s="29" t="s">
         <v>464</v>
       </c>
@@ -20762,7 +20768,7 @@
       <c r="AN125" s="19"/>
       <c r="AO125" s="20"/>
     </row>
-    <row r="126" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A126" s="29" t="s">
         <v>466</v>
       </c>
@@ -20871,7 +20877,7 @@
       <c r="AN126" s="19"/>
       <c r="AO126" s="20"/>
     </row>
-    <row r="127" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A127" s="29" t="s">
         <v>468</v>
       </c>
@@ -20980,7 +20986,7 @@
       <c r="AN127" s="19"/>
       <c r="AO127" s="20"/>
     </row>
-    <row r="128" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A128" s="29" t="s">
         <v>471</v>
       </c>
@@ -21089,7 +21095,7 @@
       <c r="AN128" s="19"/>
       <c r="AO128" s="20"/>
     </row>
-    <row r="129" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A129" s="29" t="s">
         <v>474</v>
       </c>
@@ -21198,7 +21204,7 @@
       <c r="AN129" s="19"/>
       <c r="AO129" s="20"/>
     </row>
-    <row r="130" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A130" s="29" t="s">
         <v>478</v>
       </c>
@@ -21307,7 +21313,7 @@
       <c r="AN130" s="19"/>
       <c r="AO130" s="20"/>
     </row>
-    <row r="131" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A131" s="29" t="s">
         <v>480</v>
       </c>
@@ -21416,7 +21422,7 @@
       <c r="AN131" s="19"/>
       <c r="AO131" s="20"/>
     </row>
-    <row r="132" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A132" s="29" t="s">
         <v>482</v>
       </c>
@@ -21525,7 +21531,7 @@
       <c r="AN132" s="19"/>
       <c r="AO132" s="20"/>
     </row>
-    <row r="133" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A133" s="29" t="s">
         <v>484</v>
       </c>
@@ -21634,7 +21640,7 @@
       <c r="AN133" s="19"/>
       <c r="AO133" s="20"/>
     </row>
-    <row r="134" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A134" s="29" t="s">
         <v>488</v>
       </c>
@@ -21743,7 +21749,7 @@
       <c r="AN134" s="19"/>
       <c r="AO134" s="20"/>
     </row>
-    <row r="135" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A135" s="29" t="s">
         <v>491</v>
       </c>
@@ -21852,7 +21858,7 @@
       <c r="AN135" s="19"/>
       <c r="AO135" s="20"/>
     </row>
-    <row r="136" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A136" s="29" t="s">
         <v>495</v>
       </c>
@@ -21961,7 +21967,7 @@
       <c r="AN136" s="19"/>
       <c r="AO136" s="20"/>
     </row>
-    <row r="137" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A137" s="29" t="s">
         <v>497</v>
       </c>
@@ -22070,7 +22076,7 @@
       <c r="AN137" s="19"/>
       <c r="AO137" s="20"/>
     </row>
-    <row r="138" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A138" s="29" t="s">
         <v>500</v>
       </c>
@@ -22179,7 +22185,7 @@
       <c r="AN138" s="19"/>
       <c r="AO138" s="20"/>
     </row>
-    <row r="139" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A139" s="29" t="s">
         <v>503</v>
       </c>
@@ -22288,7 +22294,7 @@
       <c r="AN139" s="19"/>
       <c r="AO139" s="20"/>
     </row>
-    <row r="140" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A140" s="29" t="s">
         <v>505</v>
       </c>
@@ -22397,7 +22403,7 @@
       <c r="AN140" s="19"/>
       <c r="AO140" s="20"/>
     </row>
-    <row r="141" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A141" s="29" t="s">
         <v>508</v>
       </c>
@@ -22506,7 +22512,7 @@
       <c r="AN141" s="19"/>
       <c r="AO141" s="20"/>
     </row>
-    <row r="142" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A142" s="29" t="s">
         <v>511</v>
       </c>
@@ -22615,7 +22621,7 @@
       <c r="AN142" s="19"/>
       <c r="AO142" s="20"/>
     </row>
-    <row r="143" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A143" s="29" t="s">
         <v>513</v>
       </c>
@@ -22724,7 +22730,7 @@
       <c r="AN143" s="19"/>
       <c r="AO143" s="20"/>
     </row>
-    <row r="144" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A144" s="29" t="s">
         <v>516</v>
       </c>
@@ -22833,7 +22839,7 @@
       <c r="AN144" s="19"/>
       <c r="AO144" s="20"/>
     </row>
-    <row r="145" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A145" s="29" t="s">
         <v>518</v>
       </c>
@@ -22942,7 +22948,7 @@
       <c r="AN145" s="19"/>
       <c r="AO145" s="20"/>
     </row>
-    <row r="146" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A146" s="29" t="s">
         <v>521</v>
       </c>
@@ -23051,7 +23057,7 @@
       <c r="AN146" s="19"/>
       <c r="AO146" s="20"/>
     </row>
-    <row r="147" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A147" s="29" t="s">
         <v>525</v>
       </c>
@@ -23160,7 +23166,7 @@
       <c r="AN147" s="19"/>
       <c r="AO147" s="20"/>
     </row>
-    <row r="148" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A148" s="29" t="s">
         <v>528</v>
       </c>
@@ -23269,7 +23275,7 @@
       <c r="AN148" s="19"/>
       <c r="AO148" s="20"/>
     </row>
-    <row r="149" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A149" s="29" t="s">
         <v>531</v>
       </c>
@@ -23378,7 +23384,7 @@
       <c r="AN149" s="19"/>
       <c r="AO149" s="20"/>
     </row>
-    <row r="150" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A150" s="29" t="s">
         <v>535</v>
       </c>
@@ -23487,7 +23493,7 @@
       <c r="AN150" s="19"/>
       <c r="AO150" s="20"/>
     </row>
-    <row r="151" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A151" s="29" t="s">
         <v>538</v>
       </c>
@@ -23598,7 +23604,7 @@
       </c>
       <c r="AO151" s="20"/>
     </row>
-    <row r="152" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A152" s="29" t="s">
         <v>541</v>
       </c>
@@ -23709,7 +23715,7 @@
       </c>
       <c r="AO152" s="20"/>
     </row>
-    <row r="153" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A153" s="29" t="s">
         <v>543</v>
       </c>
@@ -23820,7 +23826,7 @@
       </c>
       <c r="AO153" s="20"/>
     </row>
-    <row r="154" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A154" s="29" t="s">
         <v>545</v>
       </c>
@@ -23931,7 +23937,7 @@
       </c>
       <c r="AO154" s="20"/>
     </row>
-    <row r="155" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A155" s="29" t="s">
         <v>548</v>
       </c>
@@ -24040,7 +24046,7 @@
       <c r="AN155" s="19"/>
       <c r="AO155" s="20"/>
     </row>
-    <row r="156" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A156" s="29" t="s">
         <v>551</v>
       </c>
@@ -24149,7 +24155,7 @@
       <c r="AN156" s="19"/>
       <c r="AO156" s="20"/>
     </row>
-    <row r="157" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A157" s="29" t="s">
         <v>555</v>
       </c>
@@ -24258,7 +24264,7 @@
       <c r="AN157" s="19"/>
       <c r="AO157" s="20"/>
     </row>
-    <row r="158" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A158" s="29" t="s">
         <v>558</v>
       </c>
@@ -24367,7 +24373,7 @@
       <c r="AN158" s="19"/>
       <c r="AO158" s="20"/>
     </row>
-    <row r="159" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A159" s="29" t="s">
         <v>560</v>
       </c>
@@ -24476,7 +24482,7 @@
       <c r="AN159" s="19"/>
       <c r="AO159" s="20"/>
     </row>
-    <row r="160" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A160" s="29" t="s">
         <v>562</v>
       </c>
@@ -24585,7 +24591,7 @@
       <c r="AN160" s="19"/>
       <c r="AO160" s="20"/>
     </row>
-    <row r="161" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A161" s="29" t="s">
         <v>565</v>
       </c>
@@ -24694,7 +24700,7 @@
       <c r="AN161" s="19"/>
       <c r="AO161" s="20"/>
     </row>
-    <row r="162" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A162" s="29" t="s">
         <v>568</v>
       </c>
@@ -24803,7 +24809,7 @@
       <c r="AN162" s="19"/>
       <c r="AO162" s="20"/>
     </row>
-    <row r="163" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A163" s="29" t="s">
         <v>570</v>
       </c>
@@ -24912,7 +24918,7 @@
       <c r="AN163" s="19"/>
       <c r="AO163" s="20"/>
     </row>
-    <row r="164" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A164" s="29" t="s">
         <v>573</v>
       </c>
@@ -25021,7 +25027,7 @@
       <c r="AN164" s="19"/>
       <c r="AO164" s="20"/>
     </row>
-    <row r="165" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A165" s="29" t="s">
         <v>576</v>
       </c>
@@ -25130,7 +25136,7 @@
       <c r="AN165" s="19"/>
       <c r="AO165" s="20"/>
     </row>
-    <row r="166" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A166" s="29" t="s">
         <v>578</v>
       </c>
@@ -25239,7 +25245,7 @@
       <c r="AN166" s="19"/>
       <c r="AO166" s="20"/>
     </row>
-    <row r="167" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A167" s="29" t="s">
         <v>581</v>
       </c>
@@ -25350,7 +25356,7 @@
       </c>
       <c r="AO167" s="20"/>
     </row>
-    <row r="168" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A168" s="29" t="s">
         <v>585</v>
       </c>
@@ -25461,7 +25467,7 @@
       </c>
       <c r="AO168" s="20"/>
     </row>
-    <row r="169" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A169" s="29" t="s">
         <v>588</v>
       </c>
@@ -25572,7 +25578,7 @@
       </c>
       <c r="AO169" s="20"/>
     </row>
-    <row r="170" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A170" s="29" t="s">
         <v>590</v>
       </c>
@@ -25683,7 +25689,7 @@
       </c>
       <c r="AO170" s="20"/>
     </row>
-    <row r="171" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A171" s="29" t="s">
         <v>593</v>
       </c>
@@ -25792,7 +25798,7 @@
       <c r="AN171" s="19"/>
       <c r="AO171" s="20"/>
     </row>
-    <row r="172" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A172" s="29" t="s">
         <v>595</v>
       </c>
@@ -25903,7 +25909,7 @@
       </c>
       <c r="AO172" s="20"/>
     </row>
-    <row r="173" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A173" s="29" t="s">
         <v>599</v>
       </c>
@@ -26014,7 +26020,7 @@
       </c>
       <c r="AO173" s="20"/>
     </row>
-    <row r="174" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A174" s="29" t="s">
         <v>602</v>
       </c>
@@ -26125,7 +26131,7 @@
         <v>45491</v>
       </c>
     </row>
-    <row r="175" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A175" s="29" t="s">
         <v>604</v>
       </c>
@@ -26236,7 +26242,7 @@
       </c>
       <c r="AO175" s="20"/>
     </row>
-    <row r="176" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A176" s="29" t="s">
         <v>607</v>
       </c>
@@ -26347,7 +26353,7 @@
       </c>
       <c r="AO176" s="20"/>
     </row>
-    <row r="177" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A177" s="29" t="s">
         <v>610</v>
       </c>
@@ -26456,7 +26462,7 @@
       <c r="AN177" s="19"/>
       <c r="AO177" s="20"/>
     </row>
-    <row r="178" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A178" s="29" t="s">
         <v>613</v>
       </c>
@@ -26567,7 +26573,7 @@
       </c>
       <c r="AO178" s="20"/>
     </row>
-    <row r="179" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A179" s="29" t="s">
         <v>615</v>
       </c>
@@ -26678,7 +26684,7 @@
       </c>
       <c r="AO179" s="20"/>
     </row>
-    <row r="180" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A180" s="29" t="s">
         <v>618</v>
       </c>
@@ -26789,7 +26795,7 @@
       </c>
       <c r="AO180" s="20"/>
     </row>
-    <row r="181" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A181" s="29" t="s">
         <v>620</v>
       </c>
@@ -26898,7 +26904,7 @@
       <c r="AN181" s="19"/>
       <c r="AO181" s="20"/>
     </row>
-    <row r="182" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A182" s="29" t="s">
         <v>622</v>
       </c>
@@ -27009,7 +27015,7 @@
       </c>
       <c r="AO182" s="20"/>
     </row>
-    <row r="183" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A183" s="29" t="s">
         <v>624</v>
       </c>
@@ -27118,7 +27124,7 @@
       <c r="AN183" s="19"/>
       <c r="AO183" s="20"/>
     </row>
-    <row r="184" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A184" s="29" t="s">
         <v>627</v>
       </c>
@@ -27227,7 +27233,7 @@
       <c r="AN184" s="19"/>
       <c r="AO184" s="20"/>
     </row>
-    <row r="185" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A185" s="29" t="s">
         <v>630</v>
       </c>
@@ -27336,7 +27342,7 @@
       <c r="AN185" s="19"/>
       <c r="AO185" s="20"/>
     </row>
-    <row r="186" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A186" s="29" t="s">
         <v>633</v>
       </c>
@@ -27445,7 +27451,7 @@
       <c r="AN186" s="19"/>
       <c r="AO186" s="20"/>
     </row>
-    <row r="187" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A187" s="29" t="s">
         <v>636</v>
       </c>
@@ -27556,7 +27562,7 @@
       </c>
       <c r="AO187" s="20"/>
     </row>
-    <row r="188" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A188" s="29" t="s">
         <v>640</v>
       </c>
@@ -27667,7 +27673,7 @@
       </c>
       <c r="AO188" s="20"/>
     </row>
-    <row r="189" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A189" s="29" t="s">
         <v>642</v>
       </c>
@@ -27776,7 +27782,7 @@
       <c r="AN189" s="19"/>
       <c r="AO189" s="20"/>
     </row>
-    <row r="190" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A190" s="29" t="s">
         <v>646</v>
       </c>
@@ -27887,7 +27893,7 @@
       </c>
       <c r="AO190" s="20"/>
     </row>
-    <row r="191" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A191" s="29" t="s">
         <v>649</v>
       </c>
@@ -27998,7 +28004,7 @@
       </c>
       <c r="AO191" s="20"/>
     </row>
-    <row r="192" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A192" s="29" t="s">
         <v>651</v>
       </c>
@@ -28107,7 +28113,7 @@
       <c r="AN192" s="19"/>
       <c r="AO192" s="20"/>
     </row>
-    <row r="193" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A193" s="29" t="s">
         <v>655</v>
       </c>
@@ -28216,7 +28222,7 @@
       <c r="AN193" s="19"/>
       <c r="AO193" s="20"/>
     </row>
-    <row r="194" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A194" s="29" t="s">
         <v>658</v>
       </c>
@@ -28325,7 +28331,7 @@
       <c r="AN194" s="19"/>
       <c r="AO194" s="20"/>
     </row>
-    <row r="195" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A195" s="29" t="s">
         <v>662</v>
       </c>
@@ -28436,7 +28442,7 @@
       </c>
       <c r="AO195" s="20"/>
     </row>
-    <row r="196" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A196" s="29" t="s">
         <v>665</v>
       </c>
@@ -28547,7 +28553,7 @@
       </c>
       <c r="AO196" s="20"/>
     </row>
-    <row r="197" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A197" s="29" t="s">
         <v>668</v>
       </c>
@@ -28658,7 +28664,7 @@
       </c>
       <c r="AO197" s="20"/>
     </row>
-    <row r="198" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A198" s="29" t="s">
         <v>671</v>
       </c>
@@ -28777,7 +28783,7 @@
       </c>
       <c r="AO198" s="20"/>
     </row>
-    <row r="199" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A199" s="29" t="s">
         <v>675</v>
       </c>
@@ -28886,7 +28892,7 @@
       <c r="AN199" s="19"/>
       <c r="AO199" s="20"/>
     </row>
-    <row r="200" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A200" s="29" t="s">
         <v>678</v>
       </c>
@@ -28995,7 +29001,7 @@
       <c r="AN200" s="19"/>
       <c r="AO200" s="20"/>
     </row>
-    <row r="201" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A201" s="29" t="s">
         <v>682</v>
       </c>
@@ -29104,7 +29110,7 @@
       <c r="AN201" s="19"/>
       <c r="AO201" s="20"/>
     </row>
-    <row r="202" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A202" s="29" t="s">
         <v>686</v>
       </c>
@@ -29215,7 +29221,7 @@
       </c>
       <c r="AO202" s="20"/>
     </row>
-    <row r="203" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A203" s="29" t="s">
         <v>690</v>
       </c>
@@ -29324,7 +29330,7 @@
       <c r="AN203" s="19"/>
       <c r="AO203" s="20"/>
     </row>
-    <row r="204" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A204" s="29" t="s">
         <v>694</v>
       </c>
@@ -29433,7 +29439,7 @@
       <c r="AN204" s="19"/>
       <c r="AO204" s="20"/>
     </row>
-    <row r="205" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A205" s="29" t="s">
         <v>697</v>
       </c>
@@ -29542,7 +29548,7 @@
       <c r="AN205" s="19"/>
       <c r="AO205" s="20"/>
     </row>
-    <row r="206" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A206" s="29" t="s">
         <v>701</v>
       </c>
@@ -29653,7 +29659,7 @@
       </c>
       <c r="AO206" s="20"/>
     </row>
-    <row r="207" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A207" s="29" t="s">
         <v>705</v>
       </c>
@@ -29764,7 +29770,7 @@
       </c>
       <c r="AO207" s="20"/>
     </row>
-    <row r="208" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A208" s="29" t="s">
         <v>1412</v>
       </c>
@@ -29873,7 +29879,7 @@
         <v>45517</v>
       </c>
     </row>
-    <row r="209" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A209" s="29" t="s">
         <v>708</v>
       </c>
@@ -29982,7 +29988,7 @@
       <c r="AN209" s="19"/>
       <c r="AO209" s="20"/>
     </row>
-    <row r="210" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A210" s="29" t="s">
         <v>711</v>
       </c>
@@ -30091,7 +30097,7 @@
       <c r="AN210" s="19"/>
       <c r="AO210" s="20"/>
     </row>
-    <row r="211" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A211" s="29" t="s">
         <v>714</v>
       </c>
@@ -30202,7 +30208,7 @@
       </c>
       <c r="AO211" s="20"/>
     </row>
-    <row r="212" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A212" s="29" t="s">
         <v>717</v>
       </c>
@@ -30313,7 +30319,7 @@
       </c>
       <c r="AO212" s="20"/>
     </row>
-    <row r="213" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A213" s="29" t="s">
         <v>720</v>
       </c>
@@ -30424,7 +30430,7 @@
       </c>
       <c r="AO213" s="20"/>
     </row>
-    <row r="214" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A214" s="29" t="s">
         <v>723</v>
       </c>
@@ -30535,7 +30541,7 @@
       </c>
       <c r="AO214" s="20"/>
     </row>
-    <row r="215" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A215" s="29" t="s">
         <v>727</v>
       </c>
@@ -30646,7 +30652,7 @@
       </c>
       <c r="AO215" s="20"/>
     </row>
-    <row r="216" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A216" s="29" t="s">
         <v>730</v>
       </c>
@@ -30757,7 +30763,7 @@
       </c>
       <c r="AO216" s="20"/>
     </row>
-    <row r="217" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A217" s="29" t="s">
         <v>733</v>
       </c>
@@ -30868,7 +30874,7 @@
       </c>
       <c r="AO217" s="20"/>
     </row>
-    <row r="218" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A218" s="29" t="s">
         <v>736</v>
       </c>
@@ -30977,7 +30983,7 @@
       <c r="AN218" s="19"/>
       <c r="AO218" s="20"/>
     </row>
-    <row r="219" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A219" s="29" t="s">
         <v>739</v>
       </c>
@@ -31088,7 +31094,7 @@
       </c>
       <c r="AO219" s="20"/>
     </row>
-    <row r="220" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A220" s="29" t="s">
         <v>742</v>
       </c>
@@ -31197,7 +31203,7 @@
       <c r="AN220" s="19"/>
       <c r="AO220" s="20"/>
     </row>
-    <row r="221" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A221" s="29" t="s">
         <v>745</v>
       </c>
@@ -31306,7 +31312,7 @@
       <c r="AN221" s="19"/>
       <c r="AO221" s="20"/>
     </row>
-    <row r="222" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A222" s="29" t="s">
         <v>748</v>
       </c>
@@ -31415,7 +31421,7 @@
       <c r="AN222" s="19"/>
       <c r="AO222" s="20"/>
     </row>
-    <row r="223" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A223" s="29" t="s">
         <v>752</v>
       </c>
@@ -31524,7 +31530,7 @@
       <c r="AN223" s="19"/>
       <c r="AO223" s="20"/>
     </row>
-    <row r="224" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A224" s="29" t="s">
         <v>755</v>
       </c>
@@ -31633,7 +31639,7 @@
       <c r="AN224" s="19"/>
       <c r="AO224" s="20"/>
     </row>
-    <row r="225" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A225" s="29" t="s">
         <v>758</v>
       </c>
@@ -31742,7 +31748,7 @@
       <c r="AN225" s="19"/>
       <c r="AO225" s="20"/>
     </row>
-    <row r="226" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A226" s="29" t="s">
         <v>761</v>
       </c>
@@ -31853,7 +31859,7 @@
       </c>
       <c r="AO226" s="20"/>
     </row>
-    <row r="227" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A227" s="29" t="s">
         <v>764</v>
       </c>
@@ -31964,7 +31970,7 @@
       </c>
       <c r="AO227" s="20"/>
     </row>
-    <row r="228" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A228" s="29" t="s">
         <v>767</v>
       </c>
@@ -32075,7 +32081,7 @@
       </c>
       <c r="AO228" s="20"/>
     </row>
-    <row r="229" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A229" s="29" t="s">
         <v>770</v>
       </c>
@@ -32186,7 +32192,7 @@
       </c>
       <c r="AO229" s="20"/>
     </row>
-    <row r="230" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A230" s="29" t="s">
         <v>773</v>
       </c>
@@ -32295,7 +32301,7 @@
       <c r="AN230" s="19"/>
       <c r="AO230" s="20"/>
     </row>
-    <row r="231" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A231" s="29" t="s">
         <v>776</v>
       </c>
@@ -32404,7 +32410,7 @@
       <c r="AN231" s="19"/>
       <c r="AO231" s="20"/>
     </row>
-    <row r="232" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A232" s="29" t="s">
         <v>779</v>
       </c>
@@ -32513,7 +32519,7 @@
       <c r="AN232" s="19"/>
       <c r="AO232" s="20"/>
     </row>
-    <row r="233" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A233" s="29" t="s">
         <v>782</v>
       </c>
@@ -32624,7 +32630,7 @@
       </c>
       <c r="AO233" s="20"/>
     </row>
-    <row r="234" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A234" s="29" t="s">
         <v>785</v>
       </c>
@@ -32735,7 +32741,7 @@
       </c>
       <c r="AO234" s="20"/>
     </row>
-    <row r="235" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A235" s="29" t="s">
         <v>787</v>
       </c>
@@ -32846,7 +32852,7 @@
       </c>
       <c r="AO235" s="20"/>
     </row>
-    <row r="236" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A236" s="29" t="s">
         <v>790</v>
       </c>
@@ -32957,7 +32963,7 @@
       </c>
       <c r="AO236" s="20"/>
     </row>
-    <row r="237" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A237" s="29" t="s">
         <v>793</v>
       </c>
@@ -33068,7 +33074,7 @@
       </c>
       <c r="AO237" s="20"/>
     </row>
-    <row r="238" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A238" s="29" t="s">
         <v>796</v>
       </c>
@@ -33179,7 +33185,7 @@
       </c>
       <c r="AO238" s="20"/>
     </row>
-    <row r="239" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A239" s="29" t="s">
         <v>799</v>
       </c>
@@ -33290,7 +33296,7 @@
       </c>
       <c r="AO239" s="20"/>
     </row>
-    <row r="240" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A240" s="29" t="s">
         <v>803</v>
       </c>
@@ -33399,7 +33405,7 @@
       <c r="AN240" s="19"/>
       <c r="AO240" s="20"/>
     </row>
-    <row r="241" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A241" s="29" t="s">
         <v>806</v>
       </c>
@@ -33508,7 +33514,7 @@
       <c r="AN241" s="19"/>
       <c r="AO241" s="20"/>
     </row>
-    <row r="242" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A242" s="29" t="s">
         <v>809</v>
       </c>
@@ -33617,7 +33623,7 @@
       <c r="AN242" s="19"/>
       <c r="AO242" s="20"/>
     </row>
-    <row r="243" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A243" s="29" t="s">
         <v>812</v>
       </c>
@@ -33726,7 +33732,7 @@
       <c r="AN243" s="19"/>
       <c r="AO243" s="20"/>
     </row>
-    <row r="244" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A244" s="29" t="s">
         <v>816</v>
       </c>
@@ -33835,7 +33841,7 @@
       <c r="AN244" s="19"/>
       <c r="AO244" s="20"/>
     </row>
-    <row r="245" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A245" s="29" t="s">
         <v>819</v>
       </c>
@@ -33944,7 +33950,7 @@
       <c r="AN245" s="19"/>
       <c r="AO245" s="20"/>
     </row>
-    <row r="246" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A246" s="29" t="s">
         <v>822</v>
       </c>
@@ -34053,7 +34059,7 @@
       <c r="AN246" s="19"/>
       <c r="AO246" s="20"/>
     </row>
-    <row r="247" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A247" s="29" t="s">
         <v>825</v>
       </c>
@@ -34164,7 +34170,7 @@
       </c>
       <c r="AO247" s="20"/>
     </row>
-    <row r="248" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A248" s="29" t="s">
         <v>830</v>
       </c>
@@ -34273,7 +34279,7 @@
       <c r="AN248" s="23"/>
       <c r="AO248" s="20"/>
     </row>
-    <row r="249" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A249" s="29" t="s">
         <v>834</v>
       </c>
@@ -34384,7 +34390,7 @@
       </c>
       <c r="AO249" s="20"/>
     </row>
-    <row r="250" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A250" s="29" t="s">
         <v>838</v>
       </c>
@@ -34493,7 +34499,7 @@
       <c r="AN250" s="19"/>
       <c r="AO250" s="20"/>
     </row>
-    <row r="251" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A251" s="29" t="s">
         <v>841</v>
       </c>
@@ -34602,7 +34608,7 @@
       <c r="AN251" s="19"/>
       <c r="AO251" s="20"/>
     </row>
-    <row r="252" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A252" s="29" t="s">
         <v>844</v>
       </c>
@@ -34713,7 +34719,7 @@
       </c>
       <c r="AO252" s="20"/>
     </row>
-    <row r="253" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A253" s="29" t="s">
         <v>847</v>
       </c>
@@ -34824,7 +34830,7 @@
       </c>
       <c r="AO253" s="20"/>
     </row>
-    <row r="254" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A254" s="29" t="s">
         <v>849</v>
       </c>
@@ -34935,7 +34941,7 @@
       </c>
       <c r="AO254" s="20"/>
     </row>
-    <row r="255" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A255" s="29" t="s">
         <v>851</v>
       </c>
@@ -35044,7 +35050,7 @@
       <c r="AN255" s="19"/>
       <c r="AO255" s="20"/>
     </row>
-    <row r="256" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A256" s="29" t="s">
         <v>854</v>
       </c>
@@ -35155,7 +35161,7 @@
       </c>
       <c r="AO256" s="20"/>
     </row>
-    <row r="257" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A257" s="29" t="s">
         <v>857</v>
       </c>
@@ -35264,7 +35270,7 @@
       <c r="AN257" s="19"/>
       <c r="AO257" s="20"/>
     </row>
-    <row r="258" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A258" s="29" t="s">
         <v>861</v>
       </c>
@@ -35375,7 +35381,7 @@
       </c>
       <c r="AO258" s="20"/>
     </row>
-    <row r="259" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A259" s="29" t="s">
         <v>863</v>
       </c>
@@ -35488,7 +35494,7 @@
         <v>45491</v>
       </c>
     </row>
-    <row r="260" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A260" s="29" t="s">
         <v>866</v>
       </c>
@@ -35601,7 +35607,7 @@
         <v>45517</v>
       </c>
     </row>
-    <row r="261" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A261" s="29" t="s">
         <v>869</v>
       </c>
@@ -35710,7 +35716,7 @@
       <c r="AN261" s="19"/>
       <c r="AO261" s="36"/>
     </row>
-    <row r="262" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A262" s="29" t="s">
         <v>873</v>
       </c>
@@ -35821,7 +35827,7 @@
       </c>
       <c r="AO262" s="20"/>
     </row>
-    <row r="263" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A263" s="29" t="s">
         <v>877</v>
       </c>
@@ -35930,7 +35936,7 @@
       <c r="AN263" s="19"/>
       <c r="AO263" s="20"/>
     </row>
-    <row r="264" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A264" s="29" t="s">
         <v>880</v>
       </c>
@@ -36041,7 +36047,7 @@
       </c>
       <c r="AO264" s="20"/>
     </row>
-    <row r="265" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A265" s="29" t="s">
         <v>883</v>
       </c>
@@ -36154,7 +36160,7 @@
         <v>45571</v>
       </c>
     </row>
-    <row r="266" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A266" s="29" t="s">
         <v>886</v>
       </c>
@@ -36265,7 +36271,7 @@
       </c>
       <c r="AO266" s="20"/>
     </row>
-    <row r="267" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A267" s="29" t="s">
         <v>889</v>
       </c>
@@ -36378,7 +36384,7 @@
         <v>45571</v>
       </c>
     </row>
-    <row r="268" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A268" s="29" t="s">
         <v>892</v>
       </c>
@@ -36489,7 +36495,7 @@
         <v>45571</v>
       </c>
     </row>
-    <row r="269" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A269" s="29" t="s">
         <v>894</v>
       </c>
@@ -36606,7 +36612,7 @@
         <v>45571</v>
       </c>
     </row>
-    <row r="270" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A270" s="29" t="s">
         <v>897</v>
       </c>
@@ -36719,7 +36725,7 @@
         <v>45517</v>
       </c>
     </row>
-    <row r="271" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A271" s="29" t="s">
         <v>899</v>
       </c>
@@ -36832,7 +36838,7 @@
         <v>45517</v>
       </c>
     </row>
-    <row r="272" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A272" s="29" t="s">
         <v>901</v>
       </c>
@@ -36943,7 +36949,7 @@
       </c>
       <c r="AO272" s="20"/>
     </row>
-    <row r="273" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A273" s="29" t="s">
         <v>905</v>
       </c>
@@ -37054,7 +37060,7 @@
       </c>
       <c r="AO273" s="20"/>
     </row>
-    <row r="274" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A274" s="29" t="s">
         <v>909</v>
       </c>
@@ -37165,7 +37171,7 @@
       </c>
       <c r="AO274" s="20"/>
     </row>
-    <row r="275" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A275" s="29" t="s">
         <v>913</v>
       </c>
@@ -37276,7 +37282,7 @@
       </c>
       <c r="AO275" s="20"/>
     </row>
-    <row r="276" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A276" s="29" t="s">
         <v>916</v>
       </c>
@@ -37385,7 +37391,7 @@
       <c r="AN276" s="19"/>
       <c r="AO276" s="20"/>
     </row>
-    <row r="277" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A277" s="29" t="s">
         <v>919</v>
       </c>
@@ -37496,7 +37502,7 @@
       </c>
       <c r="AO277" s="20"/>
     </row>
-    <row r="278" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A278" s="29" t="s">
         <v>923</v>
       </c>
@@ -37605,7 +37611,7 @@
       <c r="AN278" s="19"/>
       <c r="AO278" s="20"/>
     </row>
-    <row r="279" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A279" s="29" t="s">
         <v>927</v>
       </c>
@@ -37714,7 +37720,7 @@
       <c r="AN279" s="19"/>
       <c r="AO279" s="20"/>
     </row>
-    <row r="280" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A280" s="29" t="s">
         <v>932</v>
       </c>
@@ -37825,7 +37831,7 @@
       </c>
       <c r="AO280" s="20"/>
     </row>
-    <row r="281" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A281" s="29" t="s">
         <v>936</v>
       </c>
@@ -37934,7 +37940,7 @@
       <c r="AN281" s="19"/>
       <c r="AO281" s="20"/>
     </row>
-    <row r="282" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A282" s="29" t="s">
         <v>939</v>
       </c>
@@ -38043,7 +38049,7 @@
       <c r="AN282" s="19"/>
       <c r="AO282" s="20"/>
     </row>
-    <row r="283" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A283" s="29" t="s">
         <v>942</v>
       </c>
@@ -38152,7 +38158,7 @@
       <c r="AN283" s="19"/>
       <c r="AO283" s="20"/>
     </row>
-    <row r="284" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A284" s="29" t="s">
         <v>945</v>
       </c>
@@ -38261,7 +38267,7 @@
       <c r="AN284" s="19"/>
       <c r="AO284" s="20"/>
     </row>
-    <row r="285" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A285" s="29" t="s">
         <v>948</v>
       </c>
@@ -38370,7 +38376,7 @@
       <c r="AN285" s="19"/>
       <c r="AO285" s="20"/>
     </row>
-    <row r="286" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A286" s="29" t="s">
         <v>952</v>
       </c>
@@ -38479,7 +38485,7 @@
       <c r="AN286" s="19"/>
       <c r="AO286" s="20"/>
     </row>
-    <row r="287" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A287" s="29" t="s">
         <v>955</v>
       </c>
@@ -38588,7 +38594,7 @@
       <c r="AN287" s="19"/>
       <c r="AO287" s="20"/>
     </row>
-    <row r="288" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A288" s="29" t="s">
         <v>957</v>
       </c>
@@ -38697,7 +38703,7 @@
       <c r="AN288" s="19"/>
       <c r="AO288" s="20"/>
     </row>
-    <row r="289" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A289" s="29" t="s">
         <v>961</v>
       </c>
@@ -38806,7 +38812,7 @@
       <c r="AN289" s="19"/>
       <c r="AO289" s="20"/>
     </row>
-    <row r="290" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A290" s="29" t="s">
         <v>964</v>
       </c>
@@ -38915,7 +38921,7 @@
       <c r="AN290" s="19"/>
       <c r="AO290" s="20"/>
     </row>
-    <row r="291" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A291" s="29" t="s">
         <v>968</v>
       </c>
@@ -39024,7 +39030,7 @@
       <c r="AN291" s="19"/>
       <c r="AO291" s="20"/>
     </row>
-    <row r="292" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A292" s="29" t="s">
         <v>971</v>
       </c>
@@ -39133,7 +39139,7 @@
       <c r="AN292" s="19"/>
       <c r="AO292" s="20"/>
     </row>
-    <row r="293" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A293" s="29" t="s">
         <v>974</v>
       </c>
@@ -39242,7 +39248,7 @@
       <c r="AN293" s="19"/>
       <c r="AO293" s="20"/>
     </row>
-    <row r="294" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A294" s="29" t="s">
         <v>977</v>
       </c>
@@ -39351,7 +39357,7 @@
       <c r="AN294" s="19"/>
       <c r="AO294" s="20"/>
     </row>
-    <row r="295" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A295" s="29" t="s">
         <v>980</v>
       </c>
@@ -39462,7 +39468,7 @@
       </c>
       <c r="AO295" s="20"/>
     </row>
-    <row r="296" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A296" s="29" t="s">
         <v>982</v>
       </c>
@@ -39573,7 +39579,7 @@
       </c>
       <c r="AO296" s="20"/>
     </row>
-    <row r="297" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A297" s="29" t="s">
         <v>985</v>
       </c>
@@ -39682,7 +39688,7 @@
       <c r="AN297" s="19"/>
       <c r="AO297" s="20"/>
     </row>
-    <row r="298" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A298" s="29" t="s">
         <v>988</v>
       </c>
@@ -39793,7 +39799,7 @@
       </c>
       <c r="AO298" s="20"/>
     </row>
-    <row r="299" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A299" s="29" t="s">
         <v>991</v>
       </c>
@@ -39904,7 +39910,7 @@
       </c>
       <c r="AO299" s="20"/>
     </row>
-    <row r="300" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A300" s="29" t="s">
         <v>993</v>
       </c>
@@ -40015,7 +40021,7 @@
       </c>
       <c r="AO300" s="20"/>
     </row>
-    <row r="301" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A301" s="29" t="s">
         <v>995</v>
       </c>
@@ -40124,7 +40130,7 @@
       <c r="AN301" s="19"/>
       <c r="AO301" s="20"/>
     </row>
-    <row r="302" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A302" s="29" t="s">
         <v>998</v>
       </c>
@@ -40233,7 +40239,7 @@
       <c r="AN302" s="19"/>
       <c r="AO302" s="20"/>
     </row>
-    <row r="303" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A303" s="29" t="s">
         <v>1001</v>
       </c>
@@ -40342,7 +40348,7 @@
       <c r="AN303" s="19"/>
       <c r="AO303" s="20"/>
     </row>
-    <row r="304" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A304" s="29" t="s">
         <v>1005</v>
       </c>
@@ -40451,7 +40457,7 @@
       <c r="AN304" s="19"/>
       <c r="AO304" s="20"/>
     </row>
-    <row r="305" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A305" s="29" t="s">
         <v>1008</v>
       </c>
@@ -40560,7 +40566,7 @@
       <c r="AN305" s="19"/>
       <c r="AO305" s="20"/>
     </row>
-    <row r="306" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A306" s="29" t="s">
         <v>1011</v>
       </c>
@@ -40671,7 +40677,7 @@
       </c>
       <c r="AO306" s="20"/>
     </row>
-    <row r="307" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A307" s="29" t="s">
         <v>1014</v>
       </c>
@@ -40780,7 +40786,7 @@
       <c r="AN307" s="19"/>
       <c r="AO307" s="20"/>
     </row>
-    <row r="308" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A308" s="29" t="s">
         <v>1017</v>
       </c>
@@ -40889,7 +40895,7 @@
       <c r="AN308" s="19"/>
       <c r="AO308" s="20"/>
     </row>
-    <row r="309" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A309" s="29" t="s">
         <v>1020</v>
       </c>
@@ -40998,7 +41004,7 @@
       <c r="AN309" s="19"/>
       <c r="AO309" s="20"/>
     </row>
-    <row r="310" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A310" s="29" t="s">
         <v>1023</v>
       </c>
@@ -41109,7 +41115,7 @@
       </c>
       <c r="AO310" s="20"/>
     </row>
-    <row r="311" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A311" s="29" t="s">
         <v>1026</v>
       </c>
@@ -41220,7 +41226,7 @@
       </c>
       <c r="AO311" s="20"/>
     </row>
-    <row r="312" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A312" s="29" t="s">
         <v>1029</v>
       </c>
@@ -41339,7 +41345,7 @@
       </c>
       <c r="AO312" s="20"/>
     </row>
-    <row r="313" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A313" s="29" t="s">
         <v>1033</v>
       </c>
@@ -41450,7 +41456,7 @@
       </c>
       <c r="AO313" s="20"/>
     </row>
-    <row r="314" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A314" s="29" t="s">
         <v>1037</v>
       </c>
@@ -41561,7 +41567,7 @@
       </c>
       <c r="AO314" s="20"/>
     </row>
-    <row r="315" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A315" s="29" t="s">
         <v>1040</v>
       </c>
@@ -41670,7 +41676,7 @@
       <c r="AN315" s="19"/>
       <c r="AO315" s="20"/>
     </row>
-    <row r="316" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A316" s="29" t="s">
         <v>1044</v>
       </c>
@@ -41779,7 +41785,7 @@
       <c r="AN316" s="19"/>
       <c r="AO316" s="20"/>
     </row>
-    <row r="317" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A317" s="29" t="s">
         <v>1048</v>
       </c>
@@ -41888,7 +41894,7 @@
       <c r="AN317" s="19"/>
       <c r="AO317" s="20"/>
     </row>
-    <row r="318" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A318" s="29" t="s">
         <v>1052</v>
       </c>
@@ -41997,7 +42003,7 @@
       <c r="AN318" s="19"/>
       <c r="AO318" s="20"/>
     </row>
-    <row r="319" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A319" s="29" t="s">
         <v>1055</v>
       </c>
@@ -42106,7 +42112,7 @@
       <c r="AN319" s="19"/>
       <c r="AO319" s="20"/>
     </row>
-    <row r="320" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A320" s="29" t="s">
         <v>1058</v>
       </c>
@@ -42215,7 +42221,7 @@
       <c r="AN320" s="19"/>
       <c r="AO320" s="20"/>
     </row>
-    <row r="321" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A321" s="29" t="s">
         <v>1061</v>
       </c>
@@ -42324,7 +42330,7 @@
       <c r="AN321" s="19"/>
       <c r="AO321" s="20"/>
     </row>
-    <row r="322" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A322" s="29" t="s">
         <v>1064</v>
       </c>
@@ -42433,7 +42439,7 @@
       <c r="AN322" s="19"/>
       <c r="AO322" s="20"/>
     </row>
-    <row r="323" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A323" s="29" t="s">
         <v>1066</v>
       </c>
@@ -42542,7 +42548,7 @@
       <c r="AN323" s="19"/>
       <c r="AO323" s="20"/>
     </row>
-    <row r="324" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A324" s="29" t="s">
         <v>1069</v>
       </c>
@@ -42651,7 +42657,7 @@
       <c r="AN324" s="19"/>
       <c r="AO324" s="20"/>
     </row>
-    <row r="325" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A325" s="29" t="s">
         <v>1072</v>
       </c>
@@ -42760,7 +42766,7 @@
       <c r="AN325" s="19"/>
       <c r="AO325" s="20"/>
     </row>
-    <row r="326" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A326" s="29" t="s">
         <v>1075</v>
       </c>
@@ -42869,7 +42875,7 @@
       <c r="AN326" s="19"/>
       <c r="AO326" s="20"/>
     </row>
-    <row r="327" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A327" s="29" t="s">
         <v>1079</v>
       </c>
@@ -42978,7 +42984,7 @@
       <c r="AN327" s="19"/>
       <c r="AO327" s="20"/>
     </row>
-    <row r="328" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A328" s="29" t="s">
         <v>1083</v>
       </c>
@@ -43087,7 +43093,7 @@
       <c r="AN328" s="19"/>
       <c r="AO328" s="20"/>
     </row>
-    <row r="329" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A329" s="29" t="s">
         <v>1087</v>
       </c>
@@ -43196,7 +43202,7 @@
       <c r="AN329" s="19"/>
       <c r="AO329" s="20"/>
     </row>
-    <row r="330" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A330" s="29" t="s">
         <v>1089</v>
       </c>
@@ -43305,7 +43311,7 @@
       <c r="AN330" s="19"/>
       <c r="AO330" s="20"/>
     </row>
-    <row r="331" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A331" s="29" t="s">
         <v>1091</v>
       </c>
@@ -43414,7 +43420,7 @@
       <c r="AN331" s="19"/>
       <c r="AO331" s="20"/>
     </row>
-    <row r="332" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A332" s="29" t="s">
         <v>1094</v>
       </c>
@@ -43523,7 +43529,7 @@
       <c r="AN332" s="19"/>
       <c r="AO332" s="20"/>
     </row>
-    <row r="333" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A333" s="29" t="s">
         <v>1096</v>
       </c>
@@ -43632,7 +43638,7 @@
       <c r="AN333" s="19"/>
       <c r="AO333" s="20"/>
     </row>
-    <row r="334" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A334" s="29" t="s">
         <v>1099</v>
       </c>
@@ -43741,7 +43747,7 @@
       <c r="AN334" s="19"/>
       <c r="AO334" s="20"/>
     </row>
-    <row r="335" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A335" s="29" t="s">
         <v>1101</v>
       </c>
@@ -43850,7 +43856,7 @@
       <c r="AN335" s="19"/>
       <c r="AO335" s="20"/>
     </row>
-    <row r="336" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A336" s="29" t="s">
         <v>1104</v>
       </c>
@@ -43959,7 +43965,7 @@
       <c r="AN336" s="19"/>
       <c r="AO336" s="20"/>
     </row>
-    <row r="337" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A337" s="29" t="s">
         <v>1107</v>
       </c>
@@ -44068,7 +44074,7 @@
       <c r="AN337" s="19"/>
       <c r="AO337" s="20"/>
     </row>
-    <row r="338" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A338" s="29" t="s">
         <v>1109</v>
       </c>
@@ -44177,7 +44183,7 @@
       <c r="AN338" s="19"/>
       <c r="AO338" s="20"/>
     </row>
-    <row r="339" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A339" s="29" t="s">
         <v>1111</v>
       </c>
@@ -44286,7 +44292,7 @@
       <c r="AN339" s="19"/>
       <c r="AO339" s="20"/>
     </row>
-    <row r="340" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A340" s="29" t="s">
         <v>1114</v>
       </c>
@@ -44395,7 +44401,7 @@
       <c r="AN340" s="19"/>
       <c r="AO340" s="20"/>
     </row>
-    <row r="341" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A341" s="29" t="s">
         <v>1117</v>
       </c>
@@ -44504,7 +44510,7 @@
       <c r="AN341" s="19"/>
       <c r="AO341" s="20"/>
     </row>
-    <row r="342" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A342" s="29" t="s">
         <v>1120</v>
       </c>
@@ -44613,7 +44619,7 @@
       <c r="AN342" s="19"/>
       <c r="AO342" s="20"/>
     </row>
-    <row r="343" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A343" s="29" t="s">
         <v>1123</v>
       </c>
@@ -44722,7 +44728,7 @@
       <c r="AN343" s="19"/>
       <c r="AO343" s="20"/>
     </row>
-    <row r="344" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A344" s="29" t="s">
         <v>1126</v>
       </c>
@@ -44831,7 +44837,7 @@
       <c r="AN344" s="19"/>
       <c r="AO344" s="20"/>
     </row>
-    <row r="345" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A345" s="29" t="s">
         <v>1128</v>
       </c>
@@ -44940,7 +44946,7 @@
       <c r="AN345" s="19"/>
       <c r="AO345" s="20"/>
     </row>
-    <row r="346" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A346" s="29" t="s">
         <v>1131</v>
       </c>
@@ -45049,7 +45055,7 @@
       <c r="AN346" s="19"/>
       <c r="AO346" s="20"/>
     </row>
-    <row r="347" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A347" s="29" t="s">
         <v>1134</v>
       </c>
@@ -45158,7 +45164,7 @@
       <c r="AN347" s="19"/>
       <c r="AO347" s="20"/>
     </row>
-    <row r="348" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A348" s="29" t="s">
         <v>1137</v>
       </c>
@@ -45267,7 +45273,7 @@
       <c r="AN348" s="19"/>
       <c r="AO348" s="20"/>
     </row>
-    <row r="349" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A349" s="29" t="s">
         <v>1140</v>
       </c>
@@ -45376,7 +45382,7 @@
       <c r="AN349" s="19"/>
       <c r="AO349" s="20"/>
     </row>
-    <row r="350" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A350" s="29" t="s">
         <v>1143</v>
       </c>
@@ -45485,7 +45491,7 @@
       <c r="AN350" s="19"/>
       <c r="AO350" s="20"/>
     </row>
-    <row r="351" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A351" s="29" t="s">
         <v>1146</v>
       </c>
@@ -45594,7 +45600,7 @@
       <c r="AN351" s="19"/>
       <c r="AO351" s="20"/>
     </row>
-    <row r="352" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A352" s="29" t="s">
         <v>1149</v>
       </c>
@@ -45703,7 +45709,7 @@
       <c r="AN352" s="19"/>
       <c r="AO352" s="20"/>
     </row>
-    <row r="353" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A353" s="29" t="s">
         <v>1152</v>
       </c>
@@ -45816,7 +45822,7 @@
         <v>45491</v>
       </c>
     </row>
-    <row r="354" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A354" s="29" t="s">
         <v>1156</v>
       </c>
@@ -45927,7 +45933,7 @@
       </c>
       <c r="AO354" s="20"/>
     </row>
-    <row r="355" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A355" s="29" t="s">
         <v>1158</v>
       </c>
@@ -46038,7 +46044,7 @@
       </c>
       <c r="AO355" s="20"/>
     </row>
-    <row r="356" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A356" s="29" t="s">
         <v>1162</v>
       </c>
@@ -46147,7 +46153,7 @@
       <c r="AN356" s="19"/>
       <c r="AO356" s="20"/>
     </row>
-    <row r="357" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A357" s="29" t="s">
         <v>1164</v>
       </c>
@@ -46256,7 +46262,7 @@
       <c r="AN357" s="19"/>
       <c r="AO357" s="20"/>
     </row>
-    <row r="358" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A358" s="29" t="s">
         <v>1166</v>
       </c>
@@ -46365,7 +46371,7 @@
       <c r="AN358" s="19"/>
       <c r="AO358" s="20"/>
     </row>
-    <row r="359" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A359" s="29" t="s">
         <v>1170</v>
       </c>
@@ -46474,7 +46480,7 @@
       <c r="AN359" s="19"/>
       <c r="AO359" s="20"/>
     </row>
-    <row r="360" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A360" s="29" t="s">
         <v>1173</v>
       </c>
@@ -46583,7 +46589,7 @@
       <c r="AN360" s="19"/>
       <c r="AO360" s="20"/>
     </row>
-    <row r="361" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A361" s="29" t="s">
         <v>1176</v>
       </c>
@@ -46692,7 +46698,7 @@
       <c r="AN361" s="19"/>
       <c r="AO361" s="20"/>
     </row>
-    <row r="362" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A362" s="29" t="s">
         <v>1179</v>
       </c>
@@ -46801,7 +46807,7 @@
       <c r="AN362" s="19"/>
       <c r="AO362" s="20"/>
     </row>
-    <row r="363" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A363" s="29" t="s">
         <v>1183</v>
       </c>
@@ -46912,7 +46918,7 @@
       </c>
       <c r="AO363" s="20"/>
     </row>
-    <row r="364" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A364" s="29" t="s">
         <v>1186</v>
       </c>
@@ -47021,7 +47027,7 @@
       <c r="AN364" s="19"/>
       <c r="AO364" s="20"/>
     </row>
-    <row r="365" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A365" s="29" t="s">
         <v>1190</v>
       </c>
@@ -47130,7 +47136,7 @@
       <c r="AN365" s="19"/>
       <c r="AO365" s="20"/>
     </row>
-    <row r="366" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A366" s="29" t="s">
         <v>1193</v>
       </c>
@@ -47239,7 +47245,7 @@
       <c r="AN366" s="19"/>
       <c r="AO366" s="20"/>
     </row>
-    <row r="367" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A367" s="29" t="s">
         <v>1197</v>
       </c>
@@ -47350,7 +47356,7 @@
       </c>
       <c r="AO367" s="20"/>
     </row>
-    <row r="368" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A368" s="29" t="s">
         <v>1200</v>
       </c>
@@ -47461,7 +47467,7 @@
       </c>
       <c r="AO368" s="20"/>
     </row>
-    <row r="369" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A369" s="29" t="s">
         <v>1203</v>
       </c>
@@ -47570,7 +47576,7 @@
       <c r="AN369" s="19"/>
       <c r="AO369" s="20"/>
     </row>
-    <row r="370" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A370" s="29" t="s">
         <v>1206</v>
       </c>
@@ -47679,7 +47685,7 @@
       <c r="AN370" s="19"/>
       <c r="AO370" s="20"/>
     </row>
-    <row r="371" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A371" s="29" t="s">
         <v>1209</v>
       </c>
@@ -47788,7 +47794,7 @@
       <c r="AN371" s="19"/>
       <c r="AO371" s="20"/>
     </row>
-    <row r="372" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A372" s="29" t="s">
         <v>1212</v>
       </c>
@@ -47897,7 +47903,7 @@
       <c r="AN372" s="19"/>
       <c r="AO372" s="20"/>
     </row>
-    <row r="373" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A373" s="29" t="s">
         <v>1215</v>
       </c>
@@ -48006,7 +48012,7 @@
       <c r="AN373" s="19"/>
       <c r="AO373" s="20"/>
     </row>
-    <row r="374" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A374" s="29" t="s">
         <v>1219</v>
       </c>
@@ -48115,7 +48121,7 @@
       <c r="AN374" s="19"/>
       <c r="AO374" s="20"/>
     </row>
-    <row r="375" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A375" s="29" t="s">
         <v>1223</v>
       </c>
@@ -48224,7 +48230,7 @@
       <c r="AN375" s="19"/>
       <c r="AO375" s="20"/>
     </row>
-    <row r="376" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A376" s="29" t="s">
         <v>1226</v>
       </c>
@@ -48333,7 +48339,7 @@
       <c r="AN376" s="19"/>
       <c r="AO376" s="20"/>
     </row>
-    <row r="377" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A377" s="29" t="s">
         <v>1229</v>
       </c>
@@ -48442,7 +48448,7 @@
       <c r="AN377" s="19"/>
       <c r="AO377" s="20"/>
     </row>
-    <row r="378" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A378" s="29" t="s">
         <v>1231</v>
       </c>
@@ -48551,7 +48557,7 @@
       <c r="AN378" s="19"/>
       <c r="AO378" s="20"/>
     </row>
-    <row r="379" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A379" s="29" t="s">
         <v>1234</v>
       </c>
@@ -48660,7 +48666,7 @@
       <c r="AN379" s="19"/>
       <c r="AO379" s="20"/>
     </row>
-    <row r="380" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A380" s="29" t="s">
         <v>1236</v>
       </c>
@@ -48769,7 +48775,7 @@
       <c r="AN380" s="19"/>
       <c r="AO380" s="20"/>
     </row>
-    <row r="381" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A381" s="29" t="s">
         <v>1238</v>
       </c>
@@ -48878,7 +48884,7 @@
       <c r="AN381" s="19"/>
       <c r="AO381" s="20"/>
     </row>
-    <row r="382" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A382" s="29" t="s">
         <v>1241</v>
       </c>
@@ -48987,7 +48993,7 @@
       <c r="AN382" s="19"/>
       <c r="AO382" s="20"/>
     </row>
-    <row r="383" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A383" s="29" t="s">
         <v>1245</v>
       </c>
@@ -49096,7 +49102,7 @@
       <c r="AN383" s="19"/>
       <c r="AO383" s="20"/>
     </row>
-    <row r="384" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A384" s="29" t="s">
         <v>1248</v>
       </c>
@@ -49205,7 +49211,7 @@
       <c r="AN384" s="19"/>
       <c r="AO384" s="20"/>
     </row>
-    <row r="385" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A385" s="29" t="s">
         <v>1250</v>
       </c>
@@ -49314,7 +49320,7 @@
       <c r="AN385" s="19"/>
       <c r="AO385" s="20"/>
     </row>
-    <row r="386" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A386" s="29" t="s">
         <v>1253</v>
       </c>
@@ -49423,7 +49429,7 @@
       <c r="AN386" s="19"/>
       <c r="AO386" s="20"/>
     </row>
-    <row r="387" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A387" s="29" t="s">
         <v>1257</v>
       </c>
@@ -49532,7 +49538,7 @@
       <c r="AN387" s="19"/>
       <c r="AO387" s="20"/>
     </row>
-    <row r="388" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A388" s="37" t="s">
         <v>1259</v>
       </c>
@@ -49643,7 +49649,7 @@
       <c r="AN388" s="24"/>
       <c r="AO388" s="20"/>
     </row>
-    <row r="389" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
       <c r="A389" s="29" t="s">
         <v>1265</v>
       </c>
@@ -49826,23 +49832,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EEFFBB1-1A6E-4B61-8EC8-F3DF1FA46298}">
   <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="36.6640625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="54.77734375" style="7" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="71.109375" style="7" customWidth="1"/>
-    <col min="5" max="5" width="52.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="64.44140625" style="7" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="1"/>
+    <col min="2" max="2" width="54.796875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="22.1328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="71.1328125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="52.46484375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="64.46484375" style="7" customWidth="1"/>
+    <col min="7" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A1" s="5" t="s">
         <v>1267</v>
       </c>
@@ -49862,7 +49868,7 @@
         <v>1272</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -49882,7 +49888,7 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
@@ -49902,7 +49908,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A4" s="10" t="s">
         <v>2</v>
       </c>
@@ -49922,7 +49928,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A5" s="10" t="s">
         <v>3</v>
       </c>
@@ -49940,7 +49946,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A6" s="10" t="s">
         <v>4</v>
       </c>
@@ -49958,7 +49964,7 @@
         <v>1287</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A7" s="10" t="s">
         <v>5</v>
       </c>
@@ -49978,7 +49984,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A8" s="10" t="s">
         <v>6</v>
       </c>
@@ -49996,7 +50002,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="47.25" x14ac:dyDescent="0.5">
       <c r="A9" s="10" t="s">
         <v>7</v>
       </c>
@@ -50016,7 +50022,7 @@
         <v>1294</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="63" x14ac:dyDescent="0.5">
       <c r="A10" s="10" t="s">
         <v>8</v>
       </c>
@@ -50036,7 +50042,7 @@
         <v>1294</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="63" x14ac:dyDescent="0.5">
       <c r="A11" s="10" t="s">
         <v>9</v>
       </c>
@@ -50056,7 +50062,7 @@
         <v>1294</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A12" s="10" t="s">
         <v>10</v>
       </c>
@@ -50076,7 +50082,7 @@
         <v>1294</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A13" s="10" t="s">
         <v>11</v>
       </c>
@@ -50096,7 +50102,7 @@
         <v>1294</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="78" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="63" x14ac:dyDescent="0.5">
       <c r="A14" s="10" t="s">
         <v>12</v>
       </c>
@@ -50114,7 +50120,7 @@
       </c>
       <c r="F14" s="14"/>
     </row>
-    <row r="15" spans="1:6" ht="78" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="63" x14ac:dyDescent="0.5">
       <c r="A15" s="10" t="s">
         <v>13</v>
       </c>
@@ -50132,7 +50138,7 @@
       </c>
       <c r="F15" s="14"/>
     </row>
-    <row r="16" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="47.25" x14ac:dyDescent="0.5">
       <c r="A16" s="10" t="s">
         <v>14</v>
       </c>
@@ -50150,7 +50156,7 @@
       </c>
       <c r="F16" s="14"/>
     </row>
-    <row r="17" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A17" s="10" t="s">
         <v>15</v>
       </c>
@@ -50168,7 +50174,7 @@
       </c>
       <c r="F17" s="14"/>
     </row>
-    <row r="18" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A18" s="10" t="s">
         <v>16</v>
       </c>
@@ -50186,7 +50192,7 @@
       </c>
       <c r="F18" s="14"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A19" s="10" t="s">
         <v>17</v>
       </c>
@@ -50202,7 +50208,7 @@
       </c>
       <c r="F19" s="14"/>
     </row>
-    <row r="20" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A20" s="10" t="s">
         <v>18</v>
       </c>
@@ -50220,7 +50226,7 @@
       </c>
       <c r="F20" s="14"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A21" s="10" t="s">
         <v>19</v>
       </c>
@@ -50238,7 +50244,7 @@
       </c>
       <c r="F21" s="14"/>
     </row>
-    <row r="22" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A22" s="10" t="s">
         <v>20</v>
       </c>
@@ -50256,7 +50262,7 @@
       </c>
       <c r="F22" s="14"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A23" s="10" t="s">
         <v>21</v>
       </c>
@@ -50274,7 +50280,7 @@
       </c>
       <c r="F23" s="14"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A24" s="10" t="s">
         <v>22</v>
       </c>
@@ -50290,7 +50296,7 @@
       </c>
       <c r="F24" s="14"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A25" s="10" t="s">
         <v>23</v>
       </c>
@@ -50306,7 +50312,7 @@
       </c>
       <c r="F25" s="14"/>
     </row>
-    <row r="26" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A26" s="10" t="s">
         <v>24</v>
       </c>
@@ -50324,7 +50330,7 @@
         <v>1327</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A27" s="10" t="s">
         <v>25</v>
       </c>
@@ -50344,7 +50350,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A28" s="10" t="s">
         <v>26</v>
       </c>
@@ -50364,7 +50370,7 @@
         <v>1294</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A29" s="10" t="s">
         <v>27</v>
       </c>
@@ -50384,7 +50390,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A30" s="10" t="s">
         <v>28</v>
       </c>
@@ -50404,7 +50410,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A31" s="10" t="s">
         <v>29</v>
       </c>
@@ -50424,7 +50430,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A32" s="10" t="s">
         <v>30</v>
       </c>
@@ -50444,7 +50450,7 @@
         <v>1343</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A33" s="10" t="s">
         <v>31</v>
       </c>
@@ -50464,7 +50470,7 @@
         <v>1347</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A34" s="10" t="s">
         <v>32</v>
       </c>
@@ -50484,7 +50490,7 @@
         <v>1349</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A35" s="10" t="s">
         <v>33</v>
       </c>
@@ -50502,7 +50508,7 @@
       </c>
       <c r="F35" s="14"/>
     </row>
-    <row r="36" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A36" s="10" t="s">
         <v>34</v>
       </c>
@@ -50522,7 +50528,7 @@
         <v>1355</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A37" s="10" t="s">
         <v>35</v>
       </c>
@@ -50542,7 +50548,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A38" s="10" t="s">
         <v>36</v>
       </c>
@@ -50562,7 +50568,7 @@
         <v>1361</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A39" s="10" t="s">
         <v>37</v>
       </c>
@@ -50582,7 +50588,7 @@
         <v>1364</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A40" s="10" t="s">
         <v>1409</v>
       </c>
@@ -50602,7 +50608,7 @@
         <v>1404</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A41" s="10" t="s">
         <v>1406</v>
       </c>
@@ -50622,7 +50628,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A43" s="5" t="s">
         <v>1365</v>
       </c>
@@ -50630,7 +50636,7 @@
         <v>1366</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A44" s="6" t="s">
         <v>47</v>
       </c>
@@ -50638,7 +50644,7 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A45" s="10" t="s">
         <v>1368</v>
       </c>
@@ -50646,10 +50652,10 @@
         <v>1369</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A46" s="15"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A47" s="5" t="s">
         <v>1370</v>
       </c>
@@ -50657,7 +50663,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A48" s="11" t="s">
         <v>1372</v>
       </c>
@@ -50665,7 +50671,7 @@
         <v>1373</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A49" s="11" t="s">
         <v>1374</v>
       </c>
@@ -50673,7 +50679,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="47.25" x14ac:dyDescent="0.5">
       <c r="A50" s="11" t="s">
         <v>1376</v>
       </c>
@@ -50681,7 +50687,7 @@
         <v>1377</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A51" s="11" t="s">
         <v>1378</v>
       </c>
@@ -50689,7 +50695,7 @@
         <v>1379</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A52" s="11" t="s">
         <v>1380</v>
       </c>
@@ -50697,7 +50703,7 @@
         <v>1381</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A53" s="11" t="s">
         <v>1382</v>
       </c>
@@ -50705,7 +50711,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A54" s="11" t="s">
         <v>1384</v>
       </c>
@@ -50713,7 +50719,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A55" s="11" t="s">
         <v>1386</v>
       </c>
@@ -50722,7 +50728,7 @@
       </c>
       <c r="C55" s="3"/>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A56" s="11" t="s">
         <v>1388</v>
       </c>
@@ -50730,7 +50736,7 @@
         <v>1389</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A58" s="5" t="s">
         <v>1390</v>
       </c>
@@ -50738,7 +50744,7 @@
         <v>1391</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A59" s="9" t="s">
         <v>1392</v>
       </c>
@@ -50746,7 +50752,7 @@
         <v>181844</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A60" s="9" t="s">
         <v>1393</v>
       </c>
@@ -50754,112 +50760,112 @@
         <v>388</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A62" s="5" t="s">
         <v>1394</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A63" s="44" t="s">
         <v>1395</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A64" s="45"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A65" s="45"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A66" s="45"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A67" s="45"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A68" s="45"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A69" s="46"/>
     </row>
-    <row r="70" spans="1:1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A70" s="44" t="s">
         <v>1396</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A71" s="45"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A72" s="45"/>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A73" s="45"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A74" s="45"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A75" s="45"/>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A76" s="45"/>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A77" s="45"/>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A78" s="45"/>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A79" s="45"/>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A80" s="45"/>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A81" s="45"/>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A82" s="45"/>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A83" s="45"/>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A84" s="45"/>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A85" s="45"/>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A86" s="45"/>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A87" s="45"/>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A88" s="45"/>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A89" s="45"/>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A90" s="45"/>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A91" s="45"/>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A92" s="45"/>
     </row>
-    <row r="93" spans="1:2" ht="87" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" ht="87" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A93" s="46"/>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A94" s="12"/>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A95" s="12"/>
       <c r="B95" s="16"/>
     </row>
@@ -50909,6 +50915,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="2624f4f0-6830-48b6-9c21-80b2613400ca" xsi:nil="true"/>
@@ -50917,15 +50932,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -51160,6 +51166,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0E9CFC5-E3D9-4ED1-BD0E-6DB50CB80DD6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15821E26-0416-43DF-8894-FB2498CD7580}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -51172,14 +51186,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="2624f4f0-6830-48b6-9c21-80b2613400ca"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0E9CFC5-E3D9-4ED1-BD0E-6DB50CB80DD6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>